<commit_message>
feat: reproducible 1.5k/40k version
</commit_message>
<xml_diff>
--- a/result/naive-p-medium/eval/scoring_template.xlsx
+++ b/result/naive-p-medium/eval/scoring_template.xlsx
@@ -278,7 +278,7 @@
     <t>accuracy</t>
   </si>
   <si>
-    <t>logical</t>
+    <t>logic</t>
   </si>
   <si>
     <t>clarity</t>
@@ -287,7 +287,7 @@
     <t>detail</t>
   </si>
   <si>
-    <t>irrelevancy</t>
+    <t>relevancy</t>
   </si>
   <si>
     <t>plausibility</t>

</xml_diff>